<commit_message>
This is Sixth day first commit.
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="199">
   <si>
     <t>S.No</t>
   </si>
@@ -601,6 +601,92 @@
   </si>
   <si>
     <t>Creation of Front Controller</t>
+  </si>
+  <si>
+    <t>Writing Test Cases to work with ProductDAO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Video of RequestParam</t>
+  </si>
+  <si>
+    <t>Creating Landing Page and Loading Static Resource</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OuSElmnstN8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qACqz8bMqSM&amp;t=1s</t>
+  </si>
+  <si>
+    <t>Craeting Master page</t>
+  </si>
+  <si>
+    <t>Creating about us and contact us pages</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zjiFBiNxdMIurl </t>
+  </si>
+  <si>
+    <t>Resolving Active Menu problem</t>
+  </si>
+  <si>
+    <t>Lopa_ERR12</t>
+  </si>
+  <si>
+    <t>Menu was not activated as page opens</t>
+  </si>
+  <si>
+    <t>follow the sequence of js file in page.jsp &lt;!-- jQuery library --&gt;
+&lt;script src="${jquery}/jquery-3.1.1.min.js"&gt;&lt;/script&gt;  
+&lt;!-- Latest compiled JavaScript --&gt; 
+&lt;script src="${js}/bootstrap.min.js"&gt;&lt;/script&gt;
+&lt;!-- Self coded js file --&gt;
+&lt;script src="${js}/myapp.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>Creating DTO,DAO classes</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=F2L24Cy4zkQ</t>
+  </si>
+  <si>
+    <t>Linking Backend with front end project</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=STi8nP7yArs&amp;t=38s</t>
+  </si>
+  <si>
+    <t>Side bar creation</t>
+  </si>
+  <si>
+    <t>refer video part03b02bof khozema</t>
+  </si>
+  <si>
+    <t>Autowired interface</t>
+  </si>
+  <si>
+    <t>10 Minutes</t>
+  </si>
+  <si>
+    <t>Creating Category DAO and DTO</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=t15lMwO7Q28</t>
+  </si>
+  <si>
+    <t>Adding Dynamic URL, Created Category DTO and DAO, Designed Products Page</t>
+  </si>
+  <si>
+    <t>Hibernate Configuration to work with H2 Database</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CV0g70poh_g&amp;t=253s</t>
+  </si>
+  <si>
+    <t>Making the project functional till view all products</t>
   </si>
 </sst>
 </file>
@@ -665,7 +751,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -721,6 +807,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -730,7 +825,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -832,6 +927,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -850,7 +949,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1133,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,20 +1765,20 @@
       <c r="B22" s="34">
         <v>42795</v>
       </c>
-      <c r="C22" s="43" t="s">
+      <c r="C22" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="45"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="47" t="s">
+      <c r="F22" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="47" t="s">
+      <c r="G22" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="49" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1685,14 +1789,14 @@
       <c r="B23" s="34">
         <v>42795</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="46"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="48"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="48"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
@@ -2182,7 +2286,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="49">
+      <c r="A46" s="43">
         <v>45</v>
       </c>
       <c r="B46" s="15">
@@ -2232,8 +2336,8 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="7">
-        <v>46</v>
+      <c r="A48" s="43">
+        <v>47</v>
       </c>
       <c r="B48" s="28">
         <v>42797</v>
@@ -2251,7 +2355,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B49" s="28">
         <v>42797</v>
@@ -2266,6 +2370,296 @@
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="12"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="43">
+        <v>49</v>
+      </c>
+      <c r="B50" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="7">
+        <v>50</v>
+      </c>
+      <c r="B51" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="43">
+        <v>51</v>
+      </c>
+      <c r="B52" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A53" s="7">
+        <v>52</v>
+      </c>
+      <c r="B53" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="43">
+        <v>53</v>
+      </c>
+      <c r="B54" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="7">
+        <v>54</v>
+      </c>
+      <c r="B55" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="43">
+        <v>55</v>
+      </c>
+      <c r="B56" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="7">
+        <v>56</v>
+      </c>
+      <c r="B57" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="43">
+        <v>57</v>
+      </c>
+      <c r="B58" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="14"/>
+      <c r="F58" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="7">
+        <v>58</v>
+      </c>
+      <c r="B59" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" s="51">
+        <v>0.16319444444444445</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="43">
+        <v>59</v>
+      </c>
+      <c r="B60" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60" s="14"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="7">
+        <v>60</v>
+      </c>
+      <c r="B61" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="43">
+        <v>61</v>
+      </c>
+      <c r="B62" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="7">
+        <v>62</v>
+      </c>
+      <c r="B63" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="43">
+        <v>63</v>
+      </c>
+      <c r="B64" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C64" s="52" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="7">
+        <v>64</v>
+      </c>
+      <c r="B65" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C65" s="52" t="s">
+        <v>198</v>
+      </c>
+      <c r="D65" s="14"/>
+      <c r="F65" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="43">
+        <v>65</v>
+      </c>
+      <c r="B66" s="15">
+        <v>42798</v>
+      </c>
+      <c r="C66" s="33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C67" s="33"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C68" s="33"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C69" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2285,18 +2679,27 @@
     <hyperlink ref="D41" r:id="rId7" display="https://www.youtube.com/watch?v=dz6hUBdJPKc"/>
     <hyperlink ref="D42:D44" r:id="rId8" display="https://www.youtube.com/watch?v=dz6hUBdJPKc"/>
     <hyperlink ref="D40" r:id="rId9" display="https://www.youtube.com/watch?v=dz6hUBdJPKc"/>
+    <hyperlink ref="D53" r:id="rId10"/>
+    <hyperlink ref="D54" r:id="rId11"/>
+    <hyperlink ref="D55" r:id="rId12"/>
+    <hyperlink ref="D56" r:id="rId13" display="https://www.youtube.com/watch?v=zjiFBiNxdMIurl"/>
+    <hyperlink ref="D57" r:id="rId14"/>
+    <hyperlink ref="D59" r:id="rId15"/>
+    <hyperlink ref="D62" r:id="rId16"/>
+    <hyperlink ref="D63" r:id="rId17"/>
+    <hyperlink ref="D64" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView topLeftCell="A12" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2459,6 +2862,17 @@
       </c>
       <c r="D12" s="12" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is Sixth day Third commit
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="202">
   <si>
     <t>S.No</t>
   </si>
@@ -687,6 +687,15 @@
   </si>
   <si>
     <t>Making the project functional till view all products</t>
+  </si>
+  <si>
+    <t>https://mvnrepository.com/artifact/junit/junit-dep/4.11</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=S9wKr2nuHHw&amp;t=25s</t>
+  </si>
+  <si>
+    <t>Project Documentation</t>
   </si>
 </sst>
 </file>
@@ -825,7 +834,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -949,11 +958,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1239,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67:C69"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2336,7 +2342,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="43">
+      <c r="A48" s="7">
         <v>47</v>
       </c>
       <c r="B48" s="28">
@@ -2372,121 +2378,142 @@
       <c r="H49" s="12"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="43">
+      <c r="A50" s="7">
         <v>49</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="28">
         <v>42798</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F50" s="1" t="s">
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12" t="s">
         <v>80</v>
       </c>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>50</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="28">
         <v>42798</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12" t="s">
         <v>93</v>
       </c>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="43">
+      <c r="A52" s="7">
         <v>51</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="28">
         <v>42798</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="E52" s="12"/>
+      <c r="F52" s="12" t="s">
         <v>81</v>
       </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
         <v>52</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="28">
         <v>42798</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="E53" s="12"/>
+      <c r="F53" s="12" t="s">
         <v>156</v>
       </c>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="43">
+      <c r="A54" s="7">
         <v>53</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="28">
         <v>42798</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="E54" s="12"/>
+      <c r="F54" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>54</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="28">
         <v>42798</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="E55" s="12"/>
+      <c r="F55" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="43">
+      <c r="A56" s="7">
         <v>55</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="28">
         <v>42798</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="F56" s="1" t="s">
+      <c r="E56" s="12"/>
+      <c r="F56" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G56" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H56" s="1" t="s">
+      <c r="H56" s="12" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2494,171 +2521,222 @@
       <c r="A57" s="7">
         <v>56</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="28">
         <v>42798</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="F57" s="1" t="s">
+      <c r="E57" s="12"/>
+      <c r="F57" s="12" t="s">
         <v>80</v>
       </c>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
     </row>
     <row r="58" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="43">
+      <c r="A58" s="7">
         <v>57</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B58" s="28">
         <v>42798</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D58" s="14"/>
-      <c r="F58" s="1" t="s">
+      <c r="D58" s="30"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12" t="s">
         <v>80</v>
       </c>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>58</v>
       </c>
-      <c r="B59" s="15">
+      <c r="B59" s="28">
         <v>42798</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="30" t="s">
         <v>188</v>
       </c>
       <c r="E59" s="51">
         <v>0.16319444444444445</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="F59" s="12" t="s">
         <v>155</v>
       </c>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="43">
+      <c r="A60" s="7">
         <v>59</v>
       </c>
-      <c r="B60" s="15">
+      <c r="B60" s="28">
         <v>42798</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D60" s="14"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="51"/>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="12" t="s">
         <v>192</v>
       </c>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>60</v>
       </c>
-      <c r="B61" s="15">
+      <c r="B61" s="28">
         <v>42798</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="E61" s="12"/>
+      <c r="F61" s="12" t="s">
         <v>81</v>
       </c>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A62" s="43">
+      <c r="A62" s="7">
         <v>61</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="28">
         <v>42798</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="D62" s="14" t="s">
+      <c r="D62" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="F62" s="1" t="s">
+      <c r="E62" s="12"/>
+      <c r="F62" s="12" t="s">
         <v>95</v>
       </c>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
     </row>
     <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>62</v>
       </c>
-      <c r="B63" s="15">
+      <c r="B63" s="28">
         <v>42798</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D63" s="14" t="s">
+      <c r="D63" s="30" t="s">
         <v>194</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="E63" s="12"/>
+      <c r="F63" s="12" t="s">
         <v>75</v>
       </c>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="43">
+      <c r="A64" s="7">
         <v>63</v>
       </c>
-      <c r="B64" s="15">
+      <c r="B64" s="28">
         <v>42798</v>
       </c>
-      <c r="C64" s="52" t="s">
+      <c r="C64" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" s="30" t="s">
         <v>197</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="E64" s="12"/>
+      <c r="F64" s="12" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
         <v>64</v>
       </c>
-      <c r="B65" s="15">
+      <c r="B65" s="28">
         <v>42798</v>
       </c>
-      <c r="C65" s="52" t="s">
+      <c r="C65" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="D65" s="14"/>
-      <c r="F65" s="1" t="s">
+      <c r="D65" s="30"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="43">
+      <c r="G65" s="12"/>
+      <c r="H65" s="12"/>
+    </row>
+    <row r="66" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A66" s="7">
         <v>65</v>
       </c>
-      <c r="B66" s="15">
+      <c r="B66" s="28">
         <v>42798</v>
       </c>
-      <c r="C66" s="33" t="s">
+      <c r="C66" s="32" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C67" s="33"/>
-    </row>
-    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D66" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="E66" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G66" s="12"/>
+      <c r="H66" s="12"/>
+    </row>
+    <row r="67" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="12">
+        <v>66</v>
+      </c>
+      <c r="B67" s="28">
+        <v>42798</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+    </row>
+    <row r="68" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C68" s="33"/>
     </row>
-    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C69" s="33"/>
     </row>
   </sheetData>
@@ -2688,9 +2766,10 @@
     <hyperlink ref="D62" r:id="rId16"/>
     <hyperlink ref="D63" r:id="rId17"/>
     <hyperlink ref="D64" r:id="rId18"/>
+    <hyperlink ref="D66" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
This is mySeventh Day first commit
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -17,6 +17,7 @@
     <sheet name="qA" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="209">
   <si>
     <t>S.No</t>
   </si>
@@ -696,6 +697,27 @@
   </si>
   <si>
     <t>Project Documentation</t>
+  </si>
+  <si>
+    <t>http://websystique.com/springmvc/spring-4-mvc-form-validation-with-hibernate-jsr-validator-resource-handling-using-annotations/</t>
+  </si>
+  <si>
+    <t>Hibernate Validation session by trainer</t>
+  </si>
+  <si>
+    <t>CRUD operation</t>
+  </si>
+  <si>
+    <t>Spring form</t>
+  </si>
+  <si>
+    <t>CRUD with Spring form insert and view with datable</t>
+  </si>
+  <si>
+    <t>Hibernate Validation dependency setup</t>
+  </si>
+  <si>
+    <t>https://docs.jboss.org/hibernate/validator/4.2/api/org/hibernate/validator/constraints/package-summary.html</t>
   </si>
 </sst>
 </file>
@@ -940,6 +962,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -957,9 +982,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1243,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1771,20 +1793,20 @@
       <c r="B22" s="34">
         <v>42795</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="49" t="s">
+      <c r="G22" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="50" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1795,14 +1817,14 @@
       <c r="B23" s="34">
         <v>42795</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="48"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="50"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="51"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
@@ -2568,7 +2590,7 @@
       <c r="D59" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="E59" s="51">
+      <c r="E59" s="45">
         <v>0.16319444444444445</v>
       </c>
       <c r="F59" s="12" t="s">
@@ -2588,7 +2610,7 @@
         <v>191</v>
       </c>
       <c r="D60" s="30"/>
-      <c r="E60" s="51"/>
+      <c r="E60" s="45"/>
       <c r="F60" s="12" t="s">
         <v>192</v>
       </c>
@@ -2733,11 +2755,107 @@
       <c r="G67" s="12"/>
       <c r="H67" s="12"/>
     </row>
-    <row r="68" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C68" s="33"/>
-    </row>
-    <row r="69" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C69" s="33"/>
+    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="7">
+        <v>67</v>
+      </c>
+      <c r="B68" s="28">
+        <v>42799</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G68" s="12"/>
+      <c r="H68" s="12"/>
+    </row>
+    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A69" s="12">
+        <v>68</v>
+      </c>
+      <c r="B69" s="28">
+        <v>42799</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G69" s="12"/>
+      <c r="H69" s="12"/>
+    </row>
+    <row r="70" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A70" s="7">
+        <v>69</v>
+      </c>
+      <c r="B70" s="28">
+        <v>42799</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G70" s="12"/>
+      <c r="H70" s="12"/>
+    </row>
+    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A71" s="12">
+        <v>70</v>
+      </c>
+      <c r="B71" s="28">
+        <v>42799</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="D71" s="12"/>
+      <c r="E71" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G71" s="12"/>
+      <c r="H71" s="12"/>
+    </row>
+    <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="7">
+        <v>71</v>
+      </c>
+      <c r="B72" s="28">
+        <v>42799</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D72" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E72" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G72" s="45"/>
+      <c r="H72" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2767,9 +2885,10 @@
     <hyperlink ref="D63" r:id="rId17"/>
     <hyperlink ref="D64" r:id="rId18"/>
     <hyperlink ref="D66" r:id="rId19"/>
+    <hyperlink ref="E72" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
This is Eight day first Commit
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -17,7 +17,6 @@
     <sheet name="qA" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="241">
   <si>
     <t>S.No</t>
   </si>
@@ -718,6 +717,112 @@
   </si>
   <si>
     <t>https://docs.jboss.org/hibernate/validator/4.2/api/org/hibernate/validator/constraints/package-summary.html</t>
+  </si>
+  <si>
+    <t>Lopa_ERR13</t>
+  </si>
+  <si>
+    <t>Lopa_ERR14</t>
+  </si>
+  <si>
+    <t>Lopa_ERR15</t>
+  </si>
+  <si>
+    <t>UnSatifiedDependency Exception</t>
+  </si>
+  <si>
+    <t>Resolved by JBOSS dependency                       &lt;dependency&gt;
+       &lt;groupId&gt;org.jboss.logging&lt;/groupId&gt;
+       &lt;artifactId&gt;jboss-logging&lt;/artifactId&gt;
+       &lt;version&gt;3.3.0.Final&lt;/version&gt;
+       &lt;/dependency&gt;</t>
+  </si>
+  <si>
+    <t>Integer field can not be @NotBlank, @NotEmpty</t>
+  </si>
+  <si>
+    <t>Annotated with @Range</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/17074611/javax-servlet-servletexception-hv000030-no-validator-could-be-found-for-type</t>
+  </si>
+  <si>
+    <t>Lopa_ERR16</t>
+  </si>
+  <si>
+    <t>How to use @Valid and @ModelAttribute</t>
+  </si>
+  <si>
+    <t>@Valid @ModelAttribute('product') Product product</t>
+  </si>
+  <si>
+    <t>ProductCRUD Page was not redirecting with Error messages</t>
+  </si>
+  <si>
+    <t>"Add the following code inside the doAction() of ProductController class
+if(result.hasErrors()) {
+    ModelAndView model1 =new ModelAndView("page");
+    model1.addObject("title","Product Management");
+    model1.addObject("userClickProductCRUD","true");
+             return model1;
+     }</t>
+  </si>
+  <si>
+    <t>Resolving not showing validation errors in ProductCRUD.jsp page</t>
+  </si>
+  <si>
+    <t>Lopa_ERR14, Lopa_ERR15, Lopa_ERR16</t>
+  </si>
+  <si>
+    <t>4.5Hrs</t>
+  </si>
+  <si>
+    <t>Image upload file dependency add</t>
+  </si>
+  <si>
+    <t>http://www.jcombat.com/spring/create-your-first-spring-web-flow-based-web-application</t>
+  </si>
+  <si>
+    <t>http://viralpatel.net/blogs/spring-mvc-multiple-file-upload-example/</t>
+  </si>
+  <si>
+    <t>http://www.springbyexample.org/examples/simple-spring-web-flow-webapp-spring-config.html</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/10847994/spring-mvc-save-uploaded-multipartfile-to-specific-folder</t>
+  </si>
+  <si>
+    <t>15 Minutes</t>
+  </si>
+  <si>
+    <t>Added backend code</t>
+  </si>
+  <si>
+    <t>Multipart Image Upload is not effecting</t>
+  </si>
+  <si>
+    <t>Lopa_ERR17</t>
+  </si>
+  <si>
+    <t>Image is not uploading</t>
+  </si>
+  <si>
+    <t>Remove @NotBlank annotation of imageUrl from product.java file</t>
+  </si>
+  <si>
+    <t>Configured form</t>
+  </si>
+  <si>
+    <t>Understanding webflow video</t>
+  </si>
+  <si>
+    <t>Modified NavBar to add Admin section</t>
+  </si>
+  <si>
+    <t>Create User DAO and DTO</t>
+  </si>
+  <si>
+    <t>5Minutes</t>
   </si>
 </sst>
 </file>
@@ -782,7 +887,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -847,6 +952,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -856,7 +970,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -982,6 +1096,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1265,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1276,14 +1397,14 @@
     <col min="1" max="1" width="5.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="43.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="61.109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1452,7 +1573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1786,7 +1907,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -2178,7 +2299,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2195,7 +2316,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>40</v>
       </c>
@@ -2218,7 +2339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>41</v>
       </c>
@@ -2241,7 +2362,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -2264,7 +2385,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
         <v>43</v>
       </c>
@@ -2339,7 +2460,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>46</v>
       </c>
@@ -2835,7 +2956,7 @@
       <c r="G71" s="12"/>
       <c r="H71" s="12"/>
     </row>
-    <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="7">
         <v>71</v>
       </c>
@@ -2856,6 +2977,240 @@
       </c>
       <c r="G72" s="45"/>
       <c r="H72" s="12"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="12">
+        <v>72</v>
+      </c>
+      <c r="B73" s="15">
+        <v>42800</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+    </row>
+    <row r="74" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" s="7">
+        <v>73</v>
+      </c>
+      <c r="B74" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C74" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H74" s="12" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="12">
+        <v>74</v>
+      </c>
+      <c r="B75" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C75" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D75" s="12"/>
+      <c r="E75" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G75" s="12"/>
+      <c r="H75" s="12"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="7">
+        <v>75</v>
+      </c>
+      <c r="B76" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G76" s="12"/>
+      <c r="H76" s="12"/>
+    </row>
+    <row r="77" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A77" s="12">
+        <v>76</v>
+      </c>
+      <c r="B77" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D77" s="12"/>
+      <c r="E77" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G77" s="12"/>
+      <c r="H77" s="12"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="7">
+        <v>77</v>
+      </c>
+      <c r="B78" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D78" s="12"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="G78" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H78" s="12" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="12">
+        <v>78</v>
+      </c>
+      <c r="B79" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C79" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F79" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="G79" s="12"/>
+      <c r="H79" s="12"/>
+    </row>
+    <row r="80" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A80" s="7">
+        <v>79</v>
+      </c>
+      <c r="B80" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C80" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D80" s="12"/>
+      <c r="E80" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G80" s="12"/>
+      <c r="H80" s="12"/>
+    </row>
+    <row r="81" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="12">
+        <v>80</v>
+      </c>
+      <c r="B81" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G81" s="12"/>
+      <c r="H81" s="12"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="7">
+        <v>81</v>
+      </c>
+      <c r="B82" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="12">
+        <v>82</v>
+      </c>
+      <c r="B83" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C83" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="D83" s="12"/>
+      <c r="E83" s="12"/>
+      <c r="F83" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G83" s="12"/>
+      <c r="H83" s="12"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="7">
+        <v>83</v>
+      </c>
+      <c r="B84" s="28">
+        <v>42800</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G84" s="12"/>
+      <c r="H84" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2894,10 +3249,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A14" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B22" sqref="B21:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3071,6 +3426,64 @@
       </c>
       <c r="C13" s="44" t="s">
         <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="52" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="C15" s="53" t="s">
+        <v>215</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="52" t="s">
+        <v>211</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="52" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is my Ninth day first commit
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="252">
   <si>
     <t>S.No</t>
   </si>
@@ -823,6 +823,39 @@
   </si>
   <si>
     <t>5Minutes</t>
+  </si>
+  <si>
+    <t>Modification of User Entity Class</t>
+  </si>
+  <si>
+    <t>Modification of UserDAOImpl class</t>
+  </si>
+  <si>
+    <t>Create UserTestCase for inset, update, delete, retrive</t>
+  </si>
+  <si>
+    <t>Product Testcase for update and delete</t>
+  </si>
+  <si>
+    <t>Run the Register page to register as supplier and customer</t>
+  </si>
+  <si>
+    <t>Create FronEndUserController class</t>
+  </si>
+  <si>
+    <t>Configuration of Webflow</t>
+  </si>
+  <si>
+    <t>Designed billing, preRegister, navbar, welcome pages</t>
+  </si>
+  <si>
+    <t>Created membershipflow.xml file</t>
+  </si>
+  <si>
+    <t>Created Address model</t>
+  </si>
+  <si>
+    <t>Created RegisterModel class</t>
   </si>
 </sst>
 </file>
@@ -1079,30 +1112,30 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1386,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H84"/>
+  <dimension ref="A1:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="E85" sqref="E85"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1914,20 +1947,20 @@
       <c r="B22" s="34">
         <v>42795</v>
       </c>
-      <c r="C22" s="46" t="s">
+      <c r="C22" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="48"/>
+      <c r="D22" s="51"/>
       <c r="E22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="50" t="s">
+      <c r="F22" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="50" t="s">
+      <c r="H22" s="53" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1938,14 +1971,14 @@
       <c r="B23" s="34">
         <v>42795</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="49"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="51"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="51"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="52"/>
+      <c r="H23" s="54"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
@@ -3211,6 +3244,208 @@
       </c>
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="12">
+        <v>84</v>
+      </c>
+      <c r="B85" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C85" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="D85" s="12"/>
+      <c r="E85" s="12"/>
+      <c r="F85" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="7">
+        <v>85</v>
+      </c>
+      <c r="B86" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C86" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="D86" s="12"/>
+      <c r="E86" s="12"/>
+      <c r="F86" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+    </row>
+    <row r="87" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="12">
+        <v>86</v>
+      </c>
+      <c r="B87" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C87" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D87" s="12"/>
+      <c r="E87" s="12"/>
+      <c r="F87" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="7">
+        <v>87</v>
+      </c>
+      <c r="B88" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C88" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="D88" s="12"/>
+      <c r="E88" s="12"/>
+      <c r="F88" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="12">
+        <v>88</v>
+      </c>
+      <c r="B89" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C89" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="D89" s="12"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G89" s="12"/>
+      <c r="H89" s="12"/>
+    </row>
+    <row r="90" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="7">
+        <v>89</v>
+      </c>
+      <c r="B90" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C90" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="D90" s="12"/>
+      <c r="E90" s="12"/>
+      <c r="F90" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G90" s="12"/>
+      <c r="H90" s="12"/>
+    </row>
+    <row r="91" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A91" s="12">
+        <v>90</v>
+      </c>
+      <c r="B91" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C91" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F91" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+    </row>
+    <row r="92" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="7">
+        <v>91</v>
+      </c>
+      <c r="B92" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C92" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="D92" s="12"/>
+      <c r="E92" s="12"/>
+      <c r="F92" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G92" s="12"/>
+      <c r="H92" s="12"/>
+    </row>
+    <row r="93" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A93" s="12">
+        <v>92</v>
+      </c>
+      <c r="B93" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C93" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="D93" s="12"/>
+      <c r="E93" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F93" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G93" s="12"/>
+      <c r="H93" s="12"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="7">
+        <v>93</v>
+      </c>
+      <c r="B94" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C94" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="D94" s="12"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G94" s="12"/>
+      <c r="H94" s="12"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" s="12">
+        <v>94</v>
+      </c>
+      <c r="B95" s="28">
+        <v>42801</v>
+      </c>
+      <c r="C95" s="12" t="s">
+        <v>251</v>
+      </c>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G95" s="12"/>
+      <c r="H95" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3429,7 +3664,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="52" t="s">
+      <c r="A14" s="46" t="s">
         <v>209</v>
       </c>
       <c r="B14" s="13" t="s">
@@ -3440,13 +3675,13 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="46" t="s">
         <v>210</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="47" t="s">
         <v>215</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -3454,18 +3689,18 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="46" t="s">
         <v>211</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="48" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="46" t="s">
         <v>217</v>
       </c>
       <c r="B17" s="13" t="s">
@@ -3476,7 +3711,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="46" t="s">
         <v>233</v>
       </c>
       <c r="B18" s="13" t="s">

</xml_diff>

<commit_message>
This is Tenth day first commit.
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -16,7 +16,7 @@
     <sheet name="error report" sheetId="2" r:id="rId2"/>
     <sheet name="qA" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="257">
   <si>
     <t>S.No</t>
   </si>
@@ -856,6 +856,21 @@
   </si>
   <si>
     <t>Created RegisterModel class</t>
+  </si>
+  <si>
+    <t>Create RegisterHandler class</t>
+  </si>
+  <si>
+    <t>Created exception.jsp page</t>
+  </si>
+  <si>
+    <t>Configured Billing page with webflow</t>
+  </si>
+  <si>
+    <t>Testing Webflow Registration page</t>
+  </si>
+  <si>
+    <t>Created Address DAO and DTO and tested</t>
   </si>
 </sst>
 </file>
@@ -1419,10 +1434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3446,6 +3461,114 @@
       </c>
       <c r="G95" s="12"/>
       <c r="H95" s="12"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="7">
+        <v>95</v>
+      </c>
+      <c r="B96" s="28">
+        <v>42802</v>
+      </c>
+      <c r="C96" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12"/>
+      <c r="F96" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G96" s="12"/>
+      <c r="H96" s="12"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="12">
+        <v>96</v>
+      </c>
+      <c r="B97" s="28">
+        <v>42802</v>
+      </c>
+      <c r="C97" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="D97" s="12"/>
+      <c r="E97" s="12"/>
+      <c r="F97" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G97" s="12"/>
+      <c r="H97" s="12"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="7">
+        <v>97</v>
+      </c>
+      <c r="B98" s="28">
+        <v>42802</v>
+      </c>
+      <c r="C98" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="D98" s="12"/>
+      <c r="E98" s="12"/>
+      <c r="F98" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G98" s="12"/>
+      <c r="H98" s="12"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="12">
+        <v>98</v>
+      </c>
+      <c r="B99" s="28">
+        <v>42802</v>
+      </c>
+      <c r="C99" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="D99" s="12"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G99" s="12"/>
+      <c r="H99" s="12"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="7">
+        <v>99</v>
+      </c>
+      <c r="B100" s="28">
+        <v>42802</v>
+      </c>
+      <c r="C100" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="12">
+        <v>100</v>
+      </c>
+      <c r="B101" s="28">
+        <v>42802</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="D101" s="12"/>
+      <c r="E101" s="12"/>
+      <c r="F101" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G101" s="12"/>
+      <c r="H101" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
This is my Eleventh day first commit.
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="261">
   <si>
     <t>S.No</t>
   </si>
@@ -871,6 +871,18 @@
   </si>
   <si>
     <t>Created Address DAO and DTO and tested</t>
+  </si>
+  <si>
+    <t>Webflow</t>
+  </si>
+  <si>
+    <t>Spring Security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cart Implementation </t>
+  </si>
+  <si>
+    <t>6hrs</t>
   </si>
 </sst>
 </file>
@@ -1434,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3569,6 +3581,78 @@
       </c>
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="7">
+        <v>101</v>
+      </c>
+      <c r="B102" s="28">
+        <v>42803</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="D102" s="12"/>
+      <c r="E102" s="12"/>
+      <c r="F102" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="G102" s="12"/>
+      <c r="H102" s="12"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="12">
+        <v>102</v>
+      </c>
+      <c r="B103" s="28">
+        <v>42803</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="G103" s="12"/>
+      <c r="H103" s="12"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="7">
+        <v>103</v>
+      </c>
+      <c r="B104" s="28">
+        <v>42803</v>
+      </c>
+      <c r="C104" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="D104" s="12"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G104" s="12"/>
+      <c r="H104" s="12"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="12">
+        <v>104</v>
+      </c>
+      <c r="B105" s="28">
+        <v>42803</v>
+      </c>
+      <c r="C105" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D105" s="12"/>
+      <c r="E105" s="12"/>
+      <c r="F105" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G105" s="12"/>
+      <c r="H105" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
This is 12th day first commit
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="270">
   <si>
     <t>S.No</t>
   </si>
@@ -883,6 +883,33 @@
   </si>
   <si>
     <t>6hrs</t>
+  </si>
+  <si>
+    <t>Single Product Page</t>
+  </si>
+  <si>
+    <t>180 Minutes</t>
+  </si>
+  <si>
+    <t>ProductCRUD Delete operation</t>
+  </si>
+  <si>
+    <t>Cart View Page</t>
+  </si>
+  <si>
+    <t>Cart DTO, DAO, DAOIMPL</t>
+  </si>
+  <si>
+    <t>CartItem DTO, DAO, DAOIMPL</t>
+  </si>
+  <si>
+    <t>Payment view page</t>
+  </si>
+  <si>
+    <t>Payment DTO</t>
+  </si>
+  <si>
+    <t>CartFlow, CartModel, CartHandler</t>
   </si>
 </sst>
 </file>
@@ -1446,10 +1473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3653,6 +3680,150 @@
       </c>
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
+    </row>
+    <row r="106" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A106" s="7">
+        <v>105</v>
+      </c>
+      <c r="B106" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C106" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D106" s="12"/>
+      <c r="E106" s="12"/>
+      <c r="F106" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="G106" s="12"/>
+      <c r="H106" s="12"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="12">
+        <v>106</v>
+      </c>
+      <c r="B107" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C107" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="D107" s="12"/>
+      <c r="E107" s="12"/>
+      <c r="F107" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G107" s="12"/>
+      <c r="H107" s="12"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="7">
+        <v>107</v>
+      </c>
+      <c r="B108" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C108" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D108" s="12"/>
+      <c r="E108" s="12"/>
+      <c r="F108" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G108" s="12"/>
+      <c r="H108" s="12"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" s="12">
+        <v>108</v>
+      </c>
+      <c r="B109" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C109" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G109" s="12"/>
+      <c r="H109" s="12"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="7">
+        <v>109</v>
+      </c>
+      <c r="B110" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C110" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="D110" s="12"/>
+      <c r="E110" s="12"/>
+      <c r="F110" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G110" s="12"/>
+      <c r="H110" s="12"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="12">
+        <v>110</v>
+      </c>
+      <c r="B111" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G111" s="12"/>
+      <c r="H111" s="12"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="7">
+        <v>111</v>
+      </c>
+      <c r="B112" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G112" s="12"/>
+      <c r="H112" s="12"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="12">
+        <v>112</v>
+      </c>
+      <c r="B113" s="28">
+        <v>42804</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G113" s="12"/>
+      <c r="H113" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
This is my 13thDay first commit
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="289">
   <si>
     <t>S.No</t>
   </si>
@@ -910,6 +910,71 @@
   </si>
   <si>
     <t>CartFlow, CartModel, CartHandler</t>
+  </si>
+  <si>
+    <t>detached object is trying to persist</t>
+  </si>
+  <si>
+    <t>Lopa_ERR18</t>
+  </si>
+  <si>
+    <t>public boolean addCartItem(CartItem ci){
+  try {
+   sessionFactory.getCurrentSession().save(ci);
+   return true;
+  } catch (Exception e) {
+   e.printStackTrace();
+   return false;
+  }
+ }         use save() method instead of persist()</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Testcase for addToCart</t>
+  </si>
+  <si>
+    <t>Payment page with spring</t>
+  </si>
+  <si>
+    <t>Payment DAO and DAOIMpl</t>
+  </si>
+  <si>
+    <t>Cart WebFlow</t>
+  </si>
+  <si>
+    <t>Billing and Shipping page</t>
+  </si>
+  <si>
+    <t>FrontEndCart Controller</t>
+  </si>
+  <si>
+    <t>Invoice page template</t>
+  </si>
+  <si>
+    <t>HandlerTypeMismatch</t>
+  </si>
+  <si>
+    <t>Lopa_ERR19</t>
+  </si>
+  <si>
+    <t>in dispatcher-servlet id="user/billing"</t>
+  </si>
+  <si>
+    <t>Property not found exception</t>
+  </si>
+  <si>
+    <t>annotate handler class with @Component</t>
+  </si>
+  <si>
+    <t>Lopa_ERR20</t>
+  </si>
+  <si>
+    <t>Cart WebFlow Testing</t>
+  </si>
+  <si>
+    <t>Lopa_ERR19, Lopa_ERR20</t>
   </si>
 </sst>
 </file>
@@ -974,7 +1039,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1030,24 +1095,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1057,7 +1104,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1160,17 +1207,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1190,6 +1227,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1473,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H113"/>
+  <dimension ref="A1:H121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2001,20 +2041,20 @@
       <c r="B22" s="34">
         <v>42795</v>
       </c>
-      <c r="C22" s="49" t="s">
+      <c r="C22" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="51"/>
+      <c r="D22" s="47"/>
       <c r="E22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="53" t="s">
+      <c r="F22" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="51" t="s">
+      <c r="G22" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="53" t="s">
+      <c r="H22" s="49" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2025,14 +2065,14 @@
       <c r="B23" s="34">
         <v>42795</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="52"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="48"/>
       <c r="E23" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="54"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="54"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="50"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
@@ -2798,7 +2838,7 @@
       <c r="D59" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="E59" s="45">
+      <c r="E59" s="44">
         <v>0.16319444444444445</v>
       </c>
       <c r="F59" s="12" t="s">
@@ -2818,7 +2858,7 @@
         <v>191</v>
       </c>
       <c r="D60" s="30"/>
-      <c r="E60" s="45"/>
+      <c r="E60" s="44"/>
       <c r="F60" s="12" t="s">
         <v>192</v>
       </c>
@@ -3062,7 +3102,7 @@
       <c r="F72" s="12" t="s">
         <v>156</v>
       </c>
-      <c r="G72" s="45"/>
+      <c r="G72" s="44"/>
       <c r="H72" s="12"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
@@ -3824,6 +3864,158 @@
       </c>
       <c r="G113" s="12"/>
       <c r="H113" s="12"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A114" s="7">
+        <v>113</v>
+      </c>
+      <c r="B114" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G114" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H114" s="12" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A115" s="12">
+        <v>114</v>
+      </c>
+      <c r="B115" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G115" s="12"/>
+      <c r="H115" s="12"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A116" s="7">
+        <v>115</v>
+      </c>
+      <c r="B116" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G116" s="12"/>
+      <c r="H116" s="12"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A117" s="12">
+        <v>116</v>
+      </c>
+      <c r="B117" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G117" s="12"/>
+      <c r="H117" s="12"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A118" s="7">
+        <v>117</v>
+      </c>
+      <c r="B118" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G118" s="12"/>
+      <c r="H118" s="12"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A119" s="12">
+        <v>118</v>
+      </c>
+      <c r="B119" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C119" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="D119" s="12"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G119" s="12"/>
+      <c r="H119" s="12"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A120" s="7">
+        <v>119</v>
+      </c>
+      <c r="B120" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C120" s="12" t="s">
+        <v>280</v>
+      </c>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G120" s="12"/>
+      <c r="H120" s="12"/>
+    </row>
+    <row r="121" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A121" s="12">
+        <v>120</v>
+      </c>
+      <c r="B121" s="28">
+        <v>42805</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D121" s="12"/>
+      <c r="E121" s="12"/>
+      <c r="F121" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G121" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H121" s="12" t="s">
+        <v>288</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3862,10 +4054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B22" sqref="B21:B22"/>
+    <sheetView topLeftCell="A15" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4006,15 +4198,16 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="21" t="s">
         <v>161</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="12" t="s">
         <v>153</v>
       </c>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A12" s="21" t="s">
@@ -4031,73 +4224,114 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="21" t="s">
         <v>183</v>
       </c>
-      <c r="C13" s="44" t="s">
+      <c r="C13" s="11" t="s">
         <v>184</v>
       </c>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="12" t="s">
         <v>213</v>
       </c>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="C15" s="47" t="s">
+      <c r="C15" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="12" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="51" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="46" t="s">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="12" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="46" t="s">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="12" t="s">
         <v>235</v>
       </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>286</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D21" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
This is my 15th day first commit
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="296">
   <si>
     <t>S.No</t>
   </si>
@@ -976,12 +976,33 @@
   <si>
     <t>Lopa_ERR19, Lopa_ERR20</t>
   </si>
+  <si>
+    <t>javax.el.ELException: Cannot convert com.health.HealthMedicineQuestBackEnd.model.Address@6f2e4f24 of type class com.health.HealthMedicineQuestBackEnd.model.Address to class java.lang.Boolean</t>
+  </si>
+  <si>
+    <t>5.5Hrs</t>
+  </si>
+  <si>
+    <t>Configuration for Project2</t>
+  </si>
+  <si>
+    <t>Displaying Hello world</t>
+  </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>Project2 Discussion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing Angular </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1028,6 +1049,12 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1104,7 +1131,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1210,6 +1237,9 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1228,8 +1258,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1513,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H121"/>
+  <dimension ref="A1:H126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2041,20 +2071,20 @@
       <c r="B22" s="34">
         <v>42795</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="47"/>
+      <c r="D22" s="48"/>
       <c r="E22" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="49" t="s">
+      <c r="F22" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="47" t="s">
+      <c r="G22" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="49" t="s">
+      <c r="H22" s="50" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2065,14 +2095,14 @@
       <c r="B23" s="34">
         <v>42795</v>
       </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="48"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="49"/>
       <c r="E23" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F23" s="50"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="50"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="51"/>
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
@@ -4015,6 +4045,70 @@
       </c>
       <c r="H121" s="12" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A122" s="7">
+        <v>121</v>
+      </c>
+      <c r="B122" s="15">
+        <v>42806</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" s="12">
+        <v>122</v>
+      </c>
+      <c r="B123" s="15">
+        <v>42806</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F123" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A124" s="7">
+        <v>123</v>
+      </c>
+      <c r="B124" s="15">
+        <v>42806</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A125" s="12">
+        <v>124</v>
+      </c>
+      <c r="B125" s="15">
+        <v>42806</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C126" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -4054,10 +4148,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A18" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4268,7 +4362,7 @@
       <c r="B16" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="45" t="s">
         <v>219</v>
       </c>
       <c r="D16" s="3"/>
@@ -4332,6 +4426,11 @@
         <v>285</v>
       </c>
       <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.3">
+      <c r="B22" s="52" t="s">
+        <v>289</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
This is my final commit of first project
</commit_message>
<xml_diff>
--- a/LOPAMUDRA_BERA.xlsx
+++ b/LOPAMUDRA_BERA.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="306">
   <si>
     <t>S.No</t>
   </si>
@@ -977,9 +977,6 @@
     <t>Lopa_ERR19, Lopa_ERR20</t>
   </si>
   <si>
-    <t>javax.el.ELException: Cannot convert com.health.HealthMedicineQuestBackEnd.model.Address@6f2e4f24 of type class com.health.HealthMedicineQuestBackEnd.model.Address to class java.lang.Boolean</t>
-  </si>
-  <si>
     <t>5.5Hrs</t>
   </si>
   <si>
@@ -995,14 +992,47 @@
     <t>Project2 Discussion</t>
   </si>
   <si>
-    <t xml:space="preserve">Testing Angular </t>
+    <t>Installation of Visual Code</t>
+  </si>
+  <si>
+    <t>Custom exception handler example</t>
+  </si>
+  <si>
+    <t>Linking angular to spring app</t>
+  </si>
+  <si>
+    <t>Error Solving</t>
+  </si>
+  <si>
+    <t>Order Invoice page</t>
+  </si>
+  <si>
+    <t>Testing Angular Application</t>
+  </si>
+  <si>
+    <t>Webflow checkout</t>
+  </si>
+  <si>
+    <t>Update Product Item</t>
+  </si>
+  <si>
+    <t>Cart Error Resolve</t>
+  </si>
+  <si>
+    <t>Lopa_ERR21</t>
+  </si>
+  <si>
+    <t>Statestate Exception in updating product item</t>
+  </si>
+  <si>
+    <t>Add the following code in side the productCRUD.jsp page within form tag  &lt;form:hidden path="productId"&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1049,12 +1079,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1131,7 +1155,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1257,9 +1281,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1543,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H126"/>
+  <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A135" sqref="A135:H135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4051,64 +4072,254 @@
       <c r="A122" s="7">
         <v>121</v>
       </c>
-      <c r="B122" s="15">
+      <c r="B122" s="28">
         <v>42806</v>
       </c>
-      <c r="C122" s="1" t="s">
+      <c r="C122" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="F122" s="1" t="s">
-        <v>290</v>
-      </c>
+      <c r="D122" s="12"/>
+      <c r="E122" s="12"/>
+      <c r="F122" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="G122" s="12"/>
+      <c r="H122" s="12"/>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123" s="12">
         <v>122</v>
       </c>
-      <c r="B123" s="15">
+      <c r="B123" s="28">
         <v>42806</v>
       </c>
-      <c r="C123" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F123" s="1" t="s">
+      <c r="C123" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="12" t="s">
         <v>138</v>
       </c>
+      <c r="G123" s="12"/>
+      <c r="H123" s="12"/>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124" s="7">
         <v>123</v>
       </c>
-      <c r="B124" s="15">
+      <c r="B124" s="28">
         <v>42806</v>
       </c>
-      <c r="C124" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F124" s="1" t="s">
+      <c r="C124" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="D124" s="12"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12" t="s">
         <v>138</v>
       </c>
+      <c r="G124" s="12"/>
+      <c r="H124" s="12"/>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125" s="12">
         <v>124</v>
       </c>
-      <c r="B125" s="15">
+      <c r="B125" s="28">
         <v>42806</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="C125" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="12" t="s">
         <v>292</v>
       </c>
-      <c r="F125" s="1" t="s">
-        <v>293</v>
-      </c>
+      <c r="G125" s="12"/>
+      <c r="H125" s="12"/>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C126" s="1" t="s">
+      <c r="A126" s="7">
+        <v>125</v>
+      </c>
+      <c r="B126" s="28">
+        <v>42806</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="D126" s="12"/>
+      <c r="E126" s="12"/>
+      <c r="F126" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G126" s="12"/>
+      <c r="H126" s="12"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A127" s="12">
+        <v>126</v>
+      </c>
+      <c r="B127" s="28">
+        <v>42806</v>
+      </c>
+      <c r="C127" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="D127" s="12"/>
+      <c r="E127" s="12"/>
+      <c r="F127" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G127" s="12"/>
+      <c r="H127" s="12"/>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A128" s="7">
+        <v>127</v>
+      </c>
+      <c r="B128" s="28">
+        <v>42807</v>
+      </c>
+      <c r="C128" s="12" t="s">
         <v>295</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>138</v>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12"/>
+      <c r="F128" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G128" s="12"/>
+      <c r="H128" s="12"/>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A129" s="12">
+        <v>128</v>
+      </c>
+      <c r="B129" s="28">
+        <v>42807</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="D129" s="12"/>
+      <c r="E129" s="12"/>
+      <c r="F129" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="G129" s="12"/>
+      <c r="H129" s="12"/>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A130" s="7">
+        <v>129</v>
+      </c>
+      <c r="B130" s="28">
+        <v>42807</v>
+      </c>
+      <c r="C130" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="D130" s="12"/>
+      <c r="E130" s="12"/>
+      <c r="F130" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G130" s="12"/>
+      <c r="H130" s="12"/>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A131" s="12">
+        <v>130</v>
+      </c>
+      <c r="B131" s="28">
+        <v>42807</v>
+      </c>
+      <c r="C131" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="D131" s="12"/>
+      <c r="E131" s="12"/>
+      <c r="F131" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G131" s="12"/>
+      <c r="H131" s="12"/>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A132" s="7">
+        <v>131</v>
+      </c>
+      <c r="B132" s="28">
+        <v>42807</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="D132" s="12"/>
+      <c r="E132" s="12"/>
+      <c r="F132" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G132" s="12"/>
+      <c r="H132" s="12"/>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A133" s="12">
+        <v>132</v>
+      </c>
+      <c r="B133" s="28">
+        <v>42807</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12"/>
+      <c r="F133" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G133" s="12"/>
+      <c r="H133" s="12"/>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A134" s="7">
+        <v>133</v>
+      </c>
+      <c r="B134" s="28">
+        <v>42808</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="D134" s="12"/>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A135" s="12">
+        <v>134</v>
+      </c>
+      <c r="B135" s="28">
+        <v>42808</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="D135" s="12"/>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="G135" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="H135" s="12" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4150,8 +4361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A16" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4427,10 +4638,17 @@
       </c>
       <c r="D21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.3">
-      <c r="B22" s="52" t="s">
-        <v>289</v>
-      </c>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>304</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="D22" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>